<commit_message>
chore: fix excel2xml testdata (#921)
</commit_message>
<xml_diff>
--- a/testdata/excel2xml/excel2xml-testdata.xlsx
+++ b/testdata/excel2xml/excel2xml-testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/dsp-tools/testdata/excel2xml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8303E5-F6DA-0649-BC84-CE04D3CAA3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE74920-DEFF-774E-A70C-C916E9D2B7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="760" windowWidth="18200" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="760" windowWidth="25520" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
     <t>??</t>
   </si>
   <si>
-    <t>-</t>
+    <t/>
   </si>
   <si>
     <t>:hasIdentifier</t>
@@ -163,6 +163,9 @@
     <t>https://en.wiktionary.org/wiki/Ῥόδος</t>
   </si>
   <si>
+    <t>https://digiliblt.uniupo.it/xtf/view?docId=dlt000521/dlt000521.xml;query=De%20taxone;brand=default</t>
+  </si>
+  <si>
     <t>https://reg-exr.com:3000</t>
   </si>
   <si>
@@ -238,6 +241,9 @@
     <t>This is an annotation to the resource Homer</t>
   </si>
   <si>
+    <t>xml</t>
+  </si>
+  <si>
     <t>isAnnotationOf</t>
   </si>
   <si>
@@ -266,9 +272,6 @@
   </si>
   <si>
     <t>Iliad Prooem ' and a single quote in xml</t>
-  </si>
-  <si>
-    <t>xml</t>
   </si>
   <si>
     <t>:hasCopyright</t>
@@ -456,9 +459,6 @@
   </si>
   <si>
     <t xml:space="preserve">    </t>
-  </si>
-  <si>
-    <t>https://digiliblt.uniupo.it/xtf/view?docId=dlt000521/dlt000521.xml;query=De%20taxone;brand=default</t>
   </si>
 </sst>
 </file>
@@ -482,6 +482,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -495,13 +501,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -650,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -686,10 +686,19 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -698,19 +707,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -740,19 +749,19 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -764,16 +773,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1081,8 +1095,8 @@
   </sheetPr>
   <dimension ref="A1:AI47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="F26" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1121,397 +1135,9 @@
     <col min="33" max="33" width="7.5" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="10.5" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="13" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="13" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="11" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="14" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="12" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="14" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="12" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="14" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="12" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="14" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="12" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="14" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="12" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="14" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="12" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="14" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="12" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="14" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="12" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="14" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="12" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="14" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="12" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="14" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="12" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="14" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="12" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="14" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="12" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="14" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="12" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="14" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="12" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="14" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="12" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="14" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="12" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="145" max="145" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="14" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="12" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="150" max="150" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="14" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="12" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="154" max="154" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="155" max="155" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="156" max="156" width="14" bestFit="1" customWidth="1"/>
-    <col min="157" max="157" width="12" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="159" max="159" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="160" max="160" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="161" max="161" width="14" bestFit="1" customWidth="1"/>
-    <col min="162" max="162" width="12" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="164" max="164" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="14" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="12" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="170" max="170" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="171" max="171" width="14" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="12" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="174" max="174" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="175" max="175" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="14" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="12" bestFit="1" customWidth="1"/>
-    <col min="178" max="178" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="179" max="179" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="180" max="180" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="14" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="12" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="184" max="184" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="185" max="185" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="14" bestFit="1" customWidth="1"/>
-    <col min="187" max="187" width="12" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="189" max="189" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="190" max="190" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="191" max="191" width="14" bestFit="1" customWidth="1"/>
-    <col min="192" max="192" width="12" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="194" max="194" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="196" max="196" width="14" bestFit="1" customWidth="1"/>
-    <col min="197" max="197" width="12" bestFit="1" customWidth="1"/>
-    <col min="198" max="198" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="199" max="199" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="14" bestFit="1" customWidth="1"/>
-    <col min="202" max="202" width="12" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="204" max="204" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="205" max="205" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="206" max="206" width="14" bestFit="1" customWidth="1"/>
-    <col min="207" max="207" width="12" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="209" max="209" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="210" max="210" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="211" max="211" width="14" bestFit="1" customWidth="1"/>
-    <col min="212" max="212" width="12" bestFit="1" customWidth="1"/>
-    <col min="213" max="213" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="214" max="214" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="215" max="215" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="14" bestFit="1" customWidth="1"/>
-    <col min="217" max="217" width="12" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="219" max="219" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="220" max="220" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="221" max="221" width="14" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="12" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="224" max="224" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="225" max="225" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="226" max="226" width="14" bestFit="1" customWidth="1"/>
-    <col min="227" max="227" width="12" bestFit="1" customWidth="1"/>
-    <col min="228" max="228" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="230" max="230" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="231" max="231" width="14" bestFit="1" customWidth="1"/>
-    <col min="232" max="232" width="12" bestFit="1" customWidth="1"/>
-    <col min="233" max="233" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="234" max="234" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="235" max="235" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="236" max="236" width="14" bestFit="1" customWidth="1"/>
-    <col min="237" max="237" width="12" bestFit="1" customWidth="1"/>
-    <col min="238" max="238" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="239" max="239" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="240" max="240" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="241" max="241" width="14" bestFit="1" customWidth="1"/>
-    <col min="242" max="242" width="12" bestFit="1" customWidth="1"/>
-    <col min="243" max="243" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="244" max="244" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="245" max="245" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="246" max="246" width="14" bestFit="1" customWidth="1"/>
-    <col min="247" max="247" width="12" bestFit="1" customWidth="1"/>
-    <col min="248" max="248" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="249" max="249" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="250" max="250" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="251" max="251" width="14" bestFit="1" customWidth="1"/>
-    <col min="252" max="252" width="12" bestFit="1" customWidth="1"/>
-    <col min="253" max="253" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="254" max="254" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="256" max="256" width="14" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="12" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="259" max="259" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="14" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="12" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="265" max="265" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="14" bestFit="1" customWidth="1"/>
-    <col min="267" max="267" width="12" bestFit="1" customWidth="1"/>
-    <col min="268" max="268" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="269" max="269" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="270" max="270" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="271" max="271" width="14" bestFit="1" customWidth="1"/>
-    <col min="272" max="272" width="12" bestFit="1" customWidth="1"/>
-    <col min="273" max="273" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="274" max="274" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="275" max="275" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="276" max="276" width="14" bestFit="1" customWidth="1"/>
-    <col min="277" max="277" width="12" bestFit="1" customWidth="1"/>
-    <col min="278" max="278" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="279" max="279" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="280" max="280" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="281" max="281" width="14" bestFit="1" customWidth="1"/>
-    <col min="282" max="282" width="12" bestFit="1" customWidth="1"/>
-    <col min="283" max="283" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="284" max="284" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="285" max="285" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="286" max="286" width="14" bestFit="1" customWidth="1"/>
-    <col min="287" max="287" width="12" bestFit="1" customWidth="1"/>
-    <col min="288" max="288" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="289" max="289" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="290" max="290" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="291" max="291" width="14" bestFit="1" customWidth="1"/>
-    <col min="292" max="292" width="12" bestFit="1" customWidth="1"/>
-    <col min="293" max="293" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="294" max="294" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="295" max="295" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="296" max="296" width="14" bestFit="1" customWidth="1"/>
-    <col min="297" max="297" width="12" bestFit="1" customWidth="1"/>
-    <col min="298" max="298" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="299" max="299" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="300" max="300" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="301" max="301" width="14" bestFit="1" customWidth="1"/>
-    <col min="302" max="302" width="12" bestFit="1" customWidth="1"/>
-    <col min="303" max="303" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="304" max="304" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="305" max="305" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="306" max="306" width="14" bestFit="1" customWidth="1"/>
-    <col min="307" max="307" width="12" bestFit="1" customWidth="1"/>
-    <col min="308" max="308" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="309" max="309" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="310" max="310" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="311" max="311" width="14" bestFit="1" customWidth="1"/>
-    <col min="312" max="312" width="12" bestFit="1" customWidth="1"/>
-    <col min="313" max="313" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="314" max="314" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="315" max="315" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="316" max="316" width="14" bestFit="1" customWidth="1"/>
-    <col min="317" max="317" width="12" bestFit="1" customWidth="1"/>
-    <col min="318" max="318" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="319" max="319" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="320" max="320" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="321" max="321" width="14" bestFit="1" customWidth="1"/>
-    <col min="322" max="322" width="12" bestFit="1" customWidth="1"/>
-    <col min="323" max="323" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="324" max="324" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="325" max="325" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="326" max="326" width="14" bestFit="1" customWidth="1"/>
-    <col min="327" max="327" width="12" bestFit="1" customWidth="1"/>
-    <col min="328" max="328" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="329" max="329" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="330" max="330" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="331" max="331" width="14" bestFit="1" customWidth="1"/>
-    <col min="332" max="332" width="12" bestFit="1" customWidth="1"/>
-    <col min="333" max="333" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="334" max="334" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="335" max="335" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="336" max="336" width="14" bestFit="1" customWidth="1"/>
-    <col min="337" max="337" width="12" bestFit="1" customWidth="1"/>
-    <col min="338" max="338" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="339" max="339" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="340" max="340" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="341" max="341" width="14" bestFit="1" customWidth="1"/>
-    <col min="342" max="342" width="12" bestFit="1" customWidth="1"/>
-    <col min="343" max="343" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="344" max="344" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="345" max="345" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="346" max="346" width="14" bestFit="1" customWidth="1"/>
-    <col min="347" max="347" width="12" bestFit="1" customWidth="1"/>
-    <col min="348" max="348" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="349" max="349" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="350" max="350" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="351" max="351" width="14" bestFit="1" customWidth="1"/>
-    <col min="352" max="352" width="12" bestFit="1" customWidth="1"/>
-    <col min="353" max="353" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="354" max="354" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="355" max="355" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="356" max="356" width="14" bestFit="1" customWidth="1"/>
-    <col min="357" max="357" width="12" bestFit="1" customWidth="1"/>
-    <col min="358" max="358" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="359" max="359" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="360" max="360" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="361" max="361" width="14" bestFit="1" customWidth="1"/>
-    <col min="362" max="362" width="12" bestFit="1" customWidth="1"/>
-    <col min="363" max="363" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="364" max="364" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="365" max="365" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="366" max="366" width="14" bestFit="1" customWidth="1"/>
-    <col min="367" max="367" width="12" bestFit="1" customWidth="1"/>
-    <col min="368" max="368" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="369" max="369" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="370" max="370" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="371" max="371" width="14" bestFit="1" customWidth="1"/>
-    <col min="372" max="372" width="12" bestFit="1" customWidth="1"/>
-    <col min="373" max="373" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="374" max="374" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="375" max="375" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="376" max="376" width="14" bestFit="1" customWidth="1"/>
-    <col min="377" max="377" width="12" bestFit="1" customWidth="1"/>
-    <col min="378" max="378" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="379" max="379" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="380" max="380" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="381" max="381" width="14" bestFit="1" customWidth="1"/>
-    <col min="382" max="382" width="12" bestFit="1" customWidth="1"/>
-    <col min="383" max="383" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="384" max="384" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="385" max="385" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="386" max="386" width="14" bestFit="1" customWidth="1"/>
-    <col min="387" max="387" width="12" bestFit="1" customWidth="1"/>
-    <col min="388" max="388" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="389" max="389" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="390" max="390" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="391" max="391" width="14" bestFit="1" customWidth="1"/>
-    <col min="392" max="392" width="12" bestFit="1" customWidth="1"/>
-    <col min="393" max="393" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="394" max="394" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="395" max="395" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="396" max="396" width="14" bestFit="1" customWidth="1"/>
-    <col min="397" max="397" width="12" bestFit="1" customWidth="1"/>
-    <col min="398" max="398" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="399" max="399" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="400" max="400" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="401" max="401" width="14" bestFit="1" customWidth="1"/>
-    <col min="402" max="402" width="12" bestFit="1" customWidth="1"/>
-    <col min="403" max="403" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="404" max="404" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="405" max="405" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="406" max="406" width="14" bestFit="1" customWidth="1"/>
-    <col min="407" max="407" width="12" bestFit="1" customWidth="1"/>
-    <col min="408" max="408" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="409" max="409" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="410" max="410" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="411" max="411" width="14" bestFit="1" customWidth="1"/>
-    <col min="412" max="412" width="12" bestFit="1" customWidth="1"/>
-    <col min="413" max="413" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="414" max="414" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="415" max="415" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="416" max="416" width="14" bestFit="1" customWidth="1"/>
-    <col min="417" max="417" width="12" bestFit="1" customWidth="1"/>
-    <col min="418" max="418" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="419" max="419" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="420" max="420" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="421" max="421" width="14" bestFit="1" customWidth="1"/>
-    <col min="422" max="422" width="12" bestFit="1" customWidth="1"/>
-    <col min="423" max="482" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1603,7 +1229,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
@@ -1629,7 +1255,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I3" s="9"/>
       <c r="J3" s="8" t="s">
         <v>36</v>
@@ -1668,21 +1294,21 @@
         <v>39</v>
       </c>
       <c r="X3" s="9"/>
-      <c r="Y3" s="8" t="s">
+      <c r="Y3" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="Z3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA3" s="8" t="s">
-        <v>39</v>
+      <c r="Z3" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA3" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="AB3" s="9"/>
       <c r="AE3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I4" s="9"/>
       <c r="J4" s="8" t="s">
         <v>43</v>
@@ -1691,196 +1317,196 @@
         <v>44</v>
       </c>
       <c r="L4" s="9"/>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="14" t="s">
         <v>45</v>
       </c>
       <c r="O4" s="8" t="s">
         <v>39</v>
       </c>
       <c r="P4" s="9"/>
-      <c r="Q4" s="42" t="s">
-        <v>140</v>
+      <c r="Q4" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="S4" s="8" t="s">
         <v>39</v>
       </c>
       <c r="T4" s="9"/>
-      <c r="U4" s="10" t="s">
-        <v>46</v>
+      <c r="U4" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="W4" s="8" t="s">
         <v>39</v>
       </c>
       <c r="X4" s="9"/>
       <c r="Y4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AA4" s="8" t="s">
         <v>39</v>
       </c>
       <c r="AB4" s="9"/>
     </row>
-    <row r="5" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I5" s="9"/>
       <c r="J5" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K5" s="8" t="s">
         <v>44</v>
       </c>
       <c r="L5" s="9"/>
-      <c r="M5" s="10" t="s">
-        <v>49</v>
+      <c r="M5" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="O5" s="8" t="s">
         <v>39</v>
       </c>
       <c r="P5" s="9"/>
-      <c r="Q5" s="13" t="s">
-        <v>50</v>
+      <c r="Q5" s="16" t="s">
+        <v>51</v>
       </c>
       <c r="S5" s="8" t="s">
         <v>39</v>
       </c>
       <c r="T5" s="9"/>
-      <c r="U5" s="14" t="s">
-        <v>51</v>
+      <c r="U5" s="17" t="s">
+        <v>52</v>
       </c>
       <c r="W5" s="8" t="s">
         <v>39</v>
       </c>
       <c r="X5" s="9"/>
-      <c r="Y5" s="13" t="s">
-        <v>52</v>
+      <c r="Y5" s="16" t="s">
+        <v>53</v>
       </c>
       <c r="AA5" s="8" t="s">
         <v>39</v>
       </c>
       <c r="AB5" s="9"/>
     </row>
-    <row r="6" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I6" s="9"/>
       <c r="J6" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>44</v>
       </c>
       <c r="L6" s="9"/>
-      <c r="M6" s="10" t="s">
-        <v>54</v>
+      <c r="M6" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>39</v>
       </c>
       <c r="P6" s="9"/>
       <c r="Q6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="S6" s="8" t="s">
         <v>39</v>
       </c>
       <c r="T6" s="9"/>
-      <c r="U6" s="14" t="s">
-        <v>56</v>
+      <c r="U6" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="W6" s="8" t="s">
         <v>39</v>
       </c>
       <c r="X6" s="9"/>
       <c r="Y6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AA6" s="8" t="s">
         <v>39</v>
       </c>
       <c r="AB6" s="9"/>
     </row>
-    <row r="7" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I7" s="9"/>
       <c r="J7" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>44</v>
       </c>
       <c r="L7" s="9"/>
-      <c r="M7" s="10" t="s">
-        <v>59</v>
+      <c r="M7" s="14" t="s">
+        <v>60</v>
       </c>
       <c r="O7" s="8" t="s">
         <v>39</v>
       </c>
       <c r="P7" s="9"/>
       <c r="Q7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="S7" s="8" t="s">
         <v>39</v>
       </c>
       <c r="T7" s="9"/>
-      <c r="U7" s="10" t="s">
-        <v>61</v>
+      <c r="U7" s="14" t="s">
+        <v>62</v>
       </c>
       <c r="W7" s="8" t="s">
         <v>39</v>
       </c>
       <c r="X7" s="9"/>
       <c r="Y7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AA7" s="8" t="s">
         <v>39</v>
       </c>
       <c r="AB7" s="9"/>
     </row>
-    <row r="8" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="K8" s="15" t="s">
+    <row r="8" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="L8" s="16"/>
-      <c r="M8" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="15"/>
-      <c r="AA8" s="15"/>
-      <c r="AB8" s="16"/>
-    </row>
-    <row r="9" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L8" s="19"/>
+      <c r="M8" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="19"/>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="18"/>
+      <c r="AB8" s="19"/>
+    </row>
+    <row r="9" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>34</v>
@@ -1895,23 +1521,23 @@
         <v>29</v>
       </c>
       <c r="AG9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I10" s="9"/>
       <c r="J10" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L10" s="9"/>
       <c r="M10" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="O10" s="8" t="s">
         <v>39</v>
@@ -1921,21 +1547,21 @@
       <c r="X10" s="9"/>
       <c r="AB10" s="9"/>
     </row>
-    <row r="11" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="16"/>
+    <row r="11" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="19"/>
       <c r="J11" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L11" s="9"/>
       <c r="M11" s="12" t="s">
@@ -1949,56 +1575,56 @@
       <c r="X11" s="9"/>
       <c r="AB11" s="9"/>
     </row>
-    <row r="12" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="22" t="s">
-        <v>76</v>
+      <c r="H12" s="25" t="s">
+        <v>78</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="22"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="22"/>
-      <c r="W12" s="22"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="25"/>
-      <c r="Z12" s="22"/>
-      <c r="AA12" s="22"/>
-      <c r="AB12" s="23"/>
-    </row>
-    <row r="13" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="26"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="25"/>
+      <c r="X12" s="26"/>
+      <c r="Y12" s="28"/>
+      <c r="Z12" s="25"/>
+      <c r="AA12" s="25"/>
+      <c r="AB12" s="26"/>
+    </row>
+    <row r="13" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I13" s="9"/>
       <c r="J13" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L13" s="9"/>
-      <c r="M13" s="26" t="s">
-        <v>78</v>
+      <c r="M13" s="29" t="s">
+        <v>80</v>
       </c>
       <c r="N13" s="8" t="s">
         <v>38</v>
@@ -2007,153 +1633,153 @@
         <v>39</v>
       </c>
       <c r="P13" s="9"/>
-      <c r="Q13" s="27"/>
+      <c r="Q13" s="30"/>
       <c r="T13" s="9"/>
-      <c r="U13" s="26"/>
+      <c r="U13" s="29"/>
       <c r="X13" s="9"/>
-      <c r="Y13" s="27"/>
+      <c r="Y13" s="30"/>
       <c r="AB13" s="9"/>
       <c r="AC13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I14" s="9"/>
       <c r="J14" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L14" s="9"/>
-      <c r="M14" s="26" t="s">
-        <v>80</v>
+      <c r="M14" s="29" t="s">
+        <v>82</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="O14" s="8" t="s">
         <v>39</v>
       </c>
       <c r="P14" s="9"/>
-      <c r="Q14" s="27"/>
+      <c r="Q14" s="30"/>
       <c r="T14" s="9"/>
-      <c r="U14" s="26"/>
+      <c r="U14" s="29"/>
       <c r="X14" s="9"/>
-      <c r="Y14" s="27"/>
+      <c r="Y14" s="30"/>
       <c r="AB14" s="9"/>
     </row>
-    <row r="15" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I15" s="9"/>
       <c r="J15" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L15" s="9"/>
-      <c r="M15" s="26" t="s">
-        <v>83</v>
+      <c r="M15" s="29" t="s">
+        <v>84</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="O15" s="8" t="s">
         <v>39</v>
       </c>
       <c r="P15" s="9"/>
-      <c r="Q15" s="27"/>
+      <c r="Q15" s="30"/>
       <c r="T15" s="9"/>
-      <c r="U15" s="26"/>
+      <c r="U15" s="29"/>
       <c r="X15" s="9"/>
-      <c r="Y15" s="27"/>
+      <c r="Y15" s="30"/>
       <c r="AB15" s="9"/>
     </row>
     <row r="16" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H16" s="15"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="K16" s="15" t="s">
+      <c r="H16" s="18"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="L16" s="16" t="s">
+      <c r="K16" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="M16" s="28" t="s">
+      <c r="L16" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="16"/>
-      <c r="U16" s="28"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="16"/>
-      <c r="Y16" s="29"/>
-      <c r="Z16" s="15"/>
-      <c r="AA16" s="15"/>
-      <c r="AB16" s="16"/>
+      <c r="M16" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="18"/>
+      <c r="S16" s="18"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="31"/>
+      <c r="V16" s="18"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="19"/>
+      <c r="Y16" s="32"/>
+      <c r="Z16" s="18"/>
+      <c r="AA16" s="18"/>
+      <c r="AB16" s="19"/>
     </row>
     <row r="17" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" s="22" t="s">
+      <c r="A17" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="B17" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="C17" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22" t="s">
+      <c r="D17" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="22"/>
+      <c r="H17" s="25"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="30"/>
-      <c r="V17" s="22"/>
-      <c r="W17" s="22"/>
-      <c r="X17" s="23"/>
-      <c r="Y17" s="22"/>
-      <c r="Z17" s="22"/>
-      <c r="AA17" s="22"/>
-      <c r="AB17" s="23"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="26"/>
+      <c r="U17" s="33"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="25"/>
+      <c r="X17" s="26"/>
+      <c r="Y17" s="25"/>
+      <c r="Z17" s="25"/>
+      <c r="AA17" s="25"/>
+      <c r="AB17" s="26"/>
     </row>
     <row r="18" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="27"/>
+      <c r="A18" s="30"/>
       <c r="I18" s="9"/>
-      <c r="J18" s="31" t="s">
-        <v>92</v>
+      <c r="J18" s="34" t="s">
+        <v>93</v>
       </c>
       <c r="K18" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L18" s="9"/>
-      <c r="M18" s="32" t="s">
-        <v>93</v>
+      <c r="M18" s="35" t="s">
+        <v>94</v>
       </c>
       <c r="N18" s="8" t="s">
         <v>38</v>
@@ -2167,58 +1793,58 @@
       <c r="AB18" s="9"/>
     </row>
     <row r="19" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="29"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="K19" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="L19" s="16"/>
-      <c r="M19" s="33" t="s">
+      <c r="A19" s="32"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="N19" s="15"/>
-      <c r="O19" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
-      <c r="S19" s="15"/>
-      <c r="T19" s="16"/>
-      <c r="U19" s="34"/>
-      <c r="V19" s="15"/>
-      <c r="W19" s="15"/>
-      <c r="X19" s="16"/>
-      <c r="Y19" s="15"/>
-      <c r="Z19" s="15"/>
-      <c r="AA19" s="15"/>
-      <c r="AB19" s="16"/>
+      <c r="K19" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="L19" s="19"/>
+      <c r="M19" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="N19" s="18"/>
+      <c r="O19" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="18"/>
+      <c r="W19" s="18"/>
+      <c r="X19" s="19"/>
+      <c r="Y19" s="18"/>
+      <c r="Z19" s="18"/>
+      <c r="AA19" s="18"/>
+      <c r="AB19" s="19"/>
     </row>
     <row r="20" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="31" t="s">
-        <v>96</v>
+      <c r="A20" s="34" t="s">
+        <v>97</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="31" t="s">
         <v>98</v>
       </c>
+      <c r="C20" s="34" t="s">
+        <v>99</v>
+      </c>
       <c r="E20" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I20" s="9"/>
       <c r="L20" s="9"/>
@@ -2229,31 +1855,31 @@
     </row>
     <row r="21" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I21" s="9"/>
-      <c r="J21" s="31" t="s">
-        <v>69</v>
+      <c r="J21" s="34" t="s">
+        <v>70</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L21" s="9"/>
-      <c r="M21" s="32" t="s">
-        <v>101</v>
+      <c r="M21" s="35" t="s">
+        <v>102</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="O21" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="R21" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="S21" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="R21" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="S21" s="8" t="s">
-        <v>102</v>
       </c>
       <c r="T21" s="9"/>
       <c r="X21" s="9"/>
@@ -2261,18 +1887,18 @@
     </row>
     <row r="22" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I22" s="9"/>
-      <c r="J22" s="31" t="s">
-        <v>104</v>
+      <c r="J22" s="34" t="s">
+        <v>105</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L22" s="9"/>
-      <c r="M22" s="32" t="s">
-        <v>106</v>
+      <c r="M22" s="35" t="s">
+        <v>107</v>
       </c>
       <c r="O22" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="P22" s="9"/>
       <c r="T22" s="9"/>
@@ -2281,18 +1907,18 @@
     </row>
     <row r="23" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I23" s="9"/>
-      <c r="J23" s="31" t="s">
-        <v>107</v>
+      <c r="J23" s="34" t="s">
+        <v>108</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L23" s="9"/>
-      <c r="M23" s="32" t="s">
-        <v>109</v>
+      <c r="M23" s="35" t="s">
+        <v>110</v>
       </c>
       <c r="O23" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="P23" s="9"/>
       <c r="T23" s="9"/>
@@ -2300,22 +1926,22 @@
       <c r="AB23" s="9"/>
     </row>
     <row r="24" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="31" t="s">
-        <v>110</v>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="34" t="s">
+        <v>111</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L24" s="9"/>
-      <c r="M24" s="32" t="s">
-        <v>73</v>
+      <c r="M24" s="35" t="s">
+        <v>75</v>
       </c>
       <c r="O24" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="P24" s="9"/>
       <c r="T24" s="9"/>
@@ -2323,58 +1949,58 @@
       <c r="AB24" s="9"/>
     </row>
     <row r="25" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="C25" s="22" t="s">
+      <c r="A25" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="D25" s="22"/>
+      <c r="C25" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="25"/>
       <c r="E25" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="22" t="s">
-        <v>76</v>
+      <c r="H25" s="25" t="s">
+        <v>78</v>
       </c>
       <c r="I25" s="9"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="22"/>
-      <c r="R25" s="22"/>
-      <c r="S25" s="22"/>
-      <c r="T25" s="23"/>
-      <c r="U25" s="30"/>
-      <c r="V25" s="22"/>
-      <c r="W25" s="22"/>
-      <c r="X25" s="23"/>
-      <c r="Y25" s="22"/>
-      <c r="Z25" s="22"/>
-      <c r="AA25" s="22"/>
-      <c r="AB25" s="23"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="25"/>
+      <c r="T25" s="26"/>
+      <c r="U25" s="33"/>
+      <c r="V25" s="25"/>
+      <c r="W25" s="25"/>
+      <c r="X25" s="26"/>
+      <c r="Y25" s="25"/>
+      <c r="Z25" s="25"/>
+      <c r="AA25" s="25"/>
+      <c r="AB25" s="26"/>
     </row>
     <row r="26" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="27"/>
+      <c r="A26" s="30"/>
       <c r="I26" s="9"/>
-      <c r="J26" s="31" t="s">
-        <v>92</v>
+      <c r="J26" s="34" t="s">
+        <v>93</v>
       </c>
       <c r="K26" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L26" s="9"/>
-      <c r="M26" s="32" t="s">
-        <v>114</v>
+      <c r="M26" s="35" t="s">
+        <v>115</v>
       </c>
       <c r="N26" s="8" t="s">
         <v>38</v>
@@ -2383,54 +2009,54 @@
         <v>39</v>
       </c>
       <c r="P26" s="9"/>
-      <c r="Q26" s="31" t="s">
-        <v>115</v>
+      <c r="Q26" s="34" t="s">
+        <v>116</v>
       </c>
       <c r="R26" s="8" t="s">
         <v>38</v>
       </c>
       <c r="S26" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="T26" s="9"/>
       <c r="X26" s="9"/>
       <c r="AB26" s="9"/>
     </row>
     <row r="27" spans="1:28" ht="171.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="27"/>
+      <c r="A27" s="30"/>
       <c r="I27" s="9"/>
-      <c r="J27" s="31" t="s">
-        <v>116</v>
+      <c r="J27" s="34" t="s">
+        <v>117</v>
       </c>
       <c r="K27" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L27" s="9"/>
-      <c r="M27" s="32" t="s">
-        <v>117</v>
+      <c r="M27" s="35" t="s">
+        <v>118</v>
       </c>
       <c r="N27" s="8" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="O27" s="8" t="s">
         <v>39</v>
       </c>
       <c r="P27" s="9"/>
-      <c r="Q27" s="31" t="s">
-        <v>118</v>
+      <c r="Q27" s="34" t="s">
+        <v>119</v>
       </c>
       <c r="R27" s="8" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="S27" s="8" t="s">
         <v>39</v>
       </c>
       <c r="T27" s="9"/>
-      <c r="U27" s="32" t="s">
-        <v>118</v>
+      <c r="U27" s="35" t="s">
+        <v>119</v>
       </c>
       <c r="V27" s="8" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="W27" s="8" t="s">
         <v>39</v>
@@ -2439,17 +2065,17 @@
       <c r="AB27" s="9"/>
     </row>
     <row r="28" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="27"/>
+      <c r="A28" s="30"/>
       <c r="I28" s="9"/>
-      <c r="J28" s="31" t="s">
-        <v>119</v>
+      <c r="J28" s="34" t="s">
+        <v>120</v>
       </c>
       <c r="K28" s="8" t="s">
         <v>44</v>
       </c>
       <c r="L28" s="9"/>
-      <c r="M28" s="32" t="s">
-        <v>120</v>
+      <c r="M28" s="35" t="s">
+        <v>121</v>
       </c>
       <c r="O28" s="8" t="s">
         <v>39</v>
@@ -2460,17 +2086,17 @@
       <c r="AB28" s="9"/>
     </row>
     <row r="29" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="27"/>
+      <c r="A29" s="30"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="31" t="s">
-        <v>121</v>
+      <c r="J29" s="34" t="s">
+        <v>122</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L29" s="9"/>
-      <c r="M29" s="32" t="s">
-        <v>123</v>
+      <c r="M29" s="35" t="s">
+        <v>124</v>
       </c>
       <c r="O29" s="8" t="s">
         <v>39</v>
@@ -2481,30 +2107,30 @@
       <c r="AB29" s="9"/>
     </row>
     <row r="30" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="27"/>
+      <c r="A30" s="30"/>
       <c r="I30" s="9"/>
-      <c r="J30" s="31" t="s">
-        <v>124</v>
+      <c r="J30" s="34" t="s">
+        <v>125</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L30" s="9"/>
-      <c r="M30" s="32" t="s">
-        <v>126</v>
+      <c r="M30" s="35" t="s">
+        <v>127</v>
       </c>
       <c r="O30" s="8" t="s">
         <v>39</v>
       </c>
       <c r="P30" s="9"/>
-      <c r="Q30" s="31" t="s">
-        <v>127</v>
+      <c r="Q30" s="34" t="s">
+        <v>128</v>
       </c>
       <c r="S30" s="8" t="s">
         <v>39</v>
       </c>
       <c r="T30" s="9"/>
-      <c r="U30" s="36">
+      <c r="U30" s="39">
         <v>2022</v>
       </c>
       <c r="W30" s="8" t="s">
@@ -2514,55 +2140,55 @@
       <c r="AB30" s="9"/>
     </row>
     <row r="31" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="29"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="K31" s="15" t="s">
+      <c r="A31" s="32"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="L31" s="16"/>
-      <c r="M31" s="37">
+      <c r="K31" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="L31" s="19"/>
+      <c r="M31" s="40">
         <v>4711</v>
       </c>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="P31" s="16"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
-      <c r="S31" s="15"/>
-      <c r="T31" s="16"/>
-      <c r="U31" s="34"/>
-      <c r="V31" s="15"/>
-      <c r="W31" s="15"/>
-      <c r="X31" s="16"/>
-      <c r="Y31" s="15"/>
-      <c r="Z31" s="15"/>
-      <c r="AA31" s="15"/>
-      <c r="AB31" s="16"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="18"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="37"/>
+      <c r="V31" s="18"/>
+      <c r="W31" s="18"/>
+      <c r="X31" s="19"/>
+      <c r="Y31" s="18"/>
+      <c r="Z31" s="18"/>
+      <c r="AA31" s="18"/>
+      <c r="AB31" s="19"/>
     </row>
     <row r="32" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D32" s="22" t="s">
         <v>133</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>134</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>34</v>
@@ -2577,17 +2203,17 @@
     <row r="33" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I33" s="9"/>
       <c r="J33" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L33" s="9"/>
       <c r="M33" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="O33" s="8" t="s">
         <v>39</v>
@@ -2597,24 +2223,24 @@
       <c r="X33" s="9"/>
       <c r="AB33" s="9"/>
       <c r="AD33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="16"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="19"/>
       <c r="J34" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L34" s="9"/>
       <c r="M34" s="12" t="s">
@@ -2625,7 +2251,7 @@
       </c>
       <c r="P34" s="9"/>
       <c r="Q34" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="S34" s="8" t="s">
         <v>39</v>
@@ -2639,62 +2265,62 @@
     </row>
     <row r="35" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="22"/>
-      <c r="Q35" s="22"/>
-      <c r="R35" s="22"/>
-      <c r="S35" s="22"/>
-      <c r="T35" s="22"/>
-      <c r="U35" s="30"/>
-      <c r="V35" s="22"/>
-      <c r="W35" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="X35" s="22"/>
-      <c r="Y35" s="22"/>
-      <c r="Z35" s="22"/>
-      <c r="AA35" s="22"/>
-      <c r="AB35" s="22"/>
+        <v>138</v>
+      </c>
+      <c r="H35" s="25"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="33"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="25"/>
+      <c r="P35" s="25"/>
+      <c r="Q35" s="25"/>
+      <c r="R35" s="25"/>
+      <c r="S35" s="25"/>
+      <c r="T35" s="25"/>
+      <c r="U35" s="33"/>
+      <c r="V35" s="25"/>
+      <c r="W35" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="X35" s="25"/>
+      <c r="Y35" s="25"/>
+      <c r="Z35" s="25"/>
+      <c r="AA35" s="25"/>
+      <c r="AB35" s="25"/>
       <c r="AC35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:30" s="38" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="38" t="s">
+    <row r="36" spans="1:30" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="D36" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="C36" s="39" t="s">
+      <c r="M36" s="44"/>
+      <c r="U36" s="44"/>
+    </row>
+    <row r="37" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" t="s">
         <v>138</v>
-      </c>
-      <c r="D36" s="38" t="s">
-        <v>136</v>
-      </c>
-      <c r="M36" s="40"/>
-      <c r="U36" s="40"/>
-    </row>
-    <row r="37" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="E37" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AD38" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2702,15 +2328,15 @@
     <row r="41" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C43" s="41"/>
+      <c r="C43" s="46"/>
     </row>
     <row r="44" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="41"/>
+      <c r="C45" s="46"/>
     </row>
     <row r="46" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="41"/>
+      <c r="C47" s="46"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
chore(xmlupload): remove lineColor key from geometry value JSON object (DEV-4132) (#1166)
</commit_message>
<xml_diff>
--- a/testdata/excel2xml/excel2xml-testdata.xlsx
+++ b/testdata/excel2xml/excel2xml-testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/dsp-tools/testdata/excel2xml/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/dsp-tools/testdata/excel2xml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE74920-DEFF-774E-A70C-C916E9D2B7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DC22B7-1B52-8B49-9009-6393276A79D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="760" windowWidth="25520" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="760" windowWidth="29080" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="140">
   <si>
     <t>id</t>
   </si>
@@ -151,9 +151,6 @@
     <t>??</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>:hasIdentifier</t>
   </si>
   <si>
@@ -353,9 +350,6 @@
   </si>
   <si>
     <t>geometry-prop</t>
-  </si>
-  <si>
-    <t>{"type": "rectangle", "lineColor": "#ff3333", "lineWidth": 2, "points": [{"x": 0.08, "y": 0.16}, {"x": 0.73, "y": 0.72}], "original_index": 0}</t>
   </si>
   <si>
     <t>isRegionOf</t>
@@ -460,12 +454,15 @@
   <si>
     <t xml:space="preserve">    </t>
   </si>
+  <si>
+    <t>{"type": "rectangle", "lineWidth": 2, "points": [{"x": 0.08, "y": 0.16}, {"x": 0.73, "y": 0.72}], "original_index": 0}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,19 +485,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -650,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -686,9 +677,6 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -707,10 +695,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -749,19 +737,13 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -776,16 +758,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1095,8 +1071,8 @@
   </sheetPr>
   <dimension ref="A1:AI47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F26" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1137,7 +1113,7 @@
     <col min="35" max="35" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1229,7 +1205,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
@@ -1255,7 +1231,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I3" s="9"/>
       <c r="J3" s="8" t="s">
         <v>36</v>
@@ -1294,219 +1270,213 @@
         <v>39</v>
       </c>
       <c r="X3" s="9"/>
-      <c r="Y3" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z3" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA3" s="13" t="s">
-        <v>42</v>
-      </c>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
       <c r="AB3" s="9"/>
       <c r="AE3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I4" s="9"/>
       <c r="J4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="L4" s="9"/>
+      <c r="M4" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="14" t="s">
+      <c r="O4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="O4" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="15" t="s">
+      <c r="S4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="T4" s="9"/>
+      <c r="U4" s="13" t="s">
         <v>46</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="T4" s="9"/>
-      <c r="U4" s="14" t="s">
-        <v>47</v>
       </c>
       <c r="W4" s="8" t="s">
         <v>39</v>
       </c>
       <c r="X4" s="9"/>
       <c r="Y4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AA4" s="8" t="s">
         <v>39</v>
       </c>
       <c r="AB4" s="9"/>
     </row>
-    <row r="5" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I5" s="9"/>
       <c r="J5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="9"/>
+      <c r="M5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="K5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="L5" s="9"/>
-      <c r="M5" s="14" t="s">
+      <c r="O5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="16" t="s">
+      <c r="S5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="T5" s="9"/>
+      <c r="U5" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="S5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="T5" s="9"/>
-      <c r="U5" s="17" t="s">
+      <c r="W5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="W5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="16" t="s">
-        <v>53</v>
-      </c>
       <c r="AA5" s="8" t="s">
         <v>39</v>
       </c>
       <c r="AB5" s="9"/>
     </row>
-    <row r="6" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I6" s="9"/>
       <c r="J6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" s="9"/>
+      <c r="M6" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>39</v>
       </c>
       <c r="P6" s="9"/>
       <c r="Q6" t="s">
+        <v>55</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="T6" s="9"/>
+      <c r="U6" s="16" t="s">
         <v>56</v>
-      </c>
-      <c r="S6" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="T6" s="9"/>
-      <c r="U6" s="17" t="s">
-        <v>57</v>
       </c>
       <c r="W6" s="8" t="s">
         <v>39</v>
       </c>
       <c r="X6" s="9"/>
       <c r="Y6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA6" s="8" t="s">
         <v>39</v>
       </c>
       <c r="AB6" s="9"/>
     </row>
-    <row r="7" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I7" s="9"/>
       <c r="J7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="13" t="s">
         <v>59</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="L7" s="9"/>
-      <c r="M7" s="14" t="s">
-        <v>60</v>
       </c>
       <c r="O7" s="8" t="s">
         <v>39</v>
       </c>
       <c r="P7" s="9"/>
       <c r="Q7" t="s">
+        <v>60</v>
+      </c>
+      <c r="S7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="T7" s="9"/>
+      <c r="U7" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="S7" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="T7" s="9"/>
-      <c r="U7" s="14" t="s">
-        <v>62</v>
       </c>
       <c r="W7" s="8" t="s">
         <v>39</v>
       </c>
       <c r="X7" s="9"/>
       <c r="Y7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB7" s="9"/>
+    </row>
+    <row r="8" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="AA7" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB7" s="9"/>
-    </row>
-    <row r="8" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="20" t="s">
+      <c r="K8" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="18"/>
+      <c r="M8" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="K8" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="L8" s="19"/>
-      <c r="M8" s="21" t="s">
+      <c r="N8" s="17"/>
+      <c r="O8" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="22"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="18"/>
+    </row>
+    <row r="9" spans="1:35" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="18"/>
-      <c r="X8" s="19"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="18"/>
-      <c r="AA8" s="18"/>
-      <c r="AB8" s="19"/>
-    </row>
-    <row r="9" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="B9" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>34</v>
@@ -1521,23 +1491,23 @@
         <v>29</v>
       </c>
       <c r="AG9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I10" s="9"/>
       <c r="J10" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L10" s="9"/>
       <c r="M10" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="O10" s="8" t="s">
         <v>39</v>
@@ -1547,21 +1517,21 @@
       <c r="X10" s="9"/>
       <c r="AB10" s="9"/>
     </row>
-    <row r="11" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="19"/>
+    <row r="11" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="18"/>
       <c r="J11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>74</v>
       </c>
       <c r="L11" s="9"/>
       <c r="M11" s="12" t="s">
@@ -1575,56 +1545,56 @@
       <c r="X11" s="9"/>
       <c r="AB11" s="9"/>
     </row>
-    <row r="12" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>77</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="25" t="s">
-        <v>78</v>
+      <c r="H12" s="24" t="s">
+        <v>77</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="26"/>
-      <c r="U12" s="27"/>
-      <c r="V12" s="25"/>
-      <c r="W12" s="25"/>
-      <c r="X12" s="26"/>
-      <c r="Y12" s="28"/>
-      <c r="Z12" s="25"/>
-      <c r="AA12" s="25"/>
-      <c r="AB12" s="26"/>
-    </row>
-    <row r="13" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="26"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="25"/>
+      <c r="Y12" s="27"/>
+      <c r="Z12" s="24"/>
+      <c r="AA12" s="24"/>
+      <c r="AB12" s="25"/>
+    </row>
+    <row r="13" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I13" s="9"/>
       <c r="J13" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L13" s="9"/>
-      <c r="M13" s="29" t="s">
-        <v>80</v>
+      <c r="M13" s="28" t="s">
+        <v>79</v>
       </c>
       <c r="N13" s="8" t="s">
         <v>38</v>
@@ -1633,153 +1603,153 @@
         <v>39</v>
       </c>
       <c r="P13" s="9"/>
-      <c r="Q13" s="30"/>
+      <c r="Q13" s="29"/>
       <c r="T13" s="9"/>
-      <c r="U13" s="29"/>
+      <c r="U13" s="28"/>
       <c r="X13" s="9"/>
-      <c r="Y13" s="30"/>
+      <c r="Y13" s="29"/>
       <c r="AB13" s="9"/>
       <c r="AC13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I14" s="9"/>
       <c r="J14" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L14" s="9"/>
-      <c r="M14" s="29" t="s">
-        <v>82</v>
+      <c r="M14" s="28" t="s">
+        <v>81</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O14" s="8" t="s">
         <v>39</v>
       </c>
       <c r="P14" s="9"/>
-      <c r="Q14" s="30"/>
+      <c r="Q14" s="29"/>
       <c r="T14" s="9"/>
-      <c r="U14" s="29"/>
+      <c r="U14" s="28"/>
       <c r="X14" s="9"/>
-      <c r="Y14" s="30"/>
+      <c r="Y14" s="29"/>
       <c r="AB14" s="9"/>
     </row>
-    <row r="15" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I15" s="9"/>
       <c r="J15" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L15" s="9"/>
-      <c r="M15" s="29" t="s">
+      <c r="M15" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="29"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="28"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="29"/>
+      <c r="AB15" s="9"/>
+    </row>
+    <row r="16" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H16" s="17"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="N15" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="O15" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="30"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="29"/>
-      <c r="X15" s="9"/>
-      <c r="Y15" s="30"/>
-      <c r="AB15" s="9"/>
-    </row>
-    <row r="16" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H16" s="18"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="18" t="s">
+      <c r="K16" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="K16" s="18" t="s">
+      <c r="L16" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="L16" s="19" t="s">
+      <c r="M16" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="M16" s="31" t="s">
+      <c r="N16" s="17"/>
+      <c r="O16" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="18"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="18"/>
+      <c r="Y16" s="31"/>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="17"/>
+      <c r="AB16" s="18"/>
+    </row>
+    <row r="17" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="19"/>
-      <c r="U16" s="31"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="19"/>
-      <c r="Y16" s="32"/>
-      <c r="Z16" s="18"/>
-      <c r="AA16" s="18"/>
-      <c r="AB16" s="19"/>
-    </row>
-    <row r="17" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
+      <c r="B17" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="C17" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="D17" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="24"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="32"/>
+      <c r="V17" s="24"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="25"/>
+      <c r="Y17" s="24"/>
+      <c r="Z17" s="24"/>
+      <c r="AA17" s="24"/>
+      <c r="AB17" s="25"/>
+    </row>
+    <row r="18" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="29"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="14" t="s">
         <v>92</v>
-      </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="26"/>
-      <c r="U17" s="33"/>
-      <c r="V17" s="25"/>
-      <c r="W17" s="25"/>
-      <c r="X17" s="26"/>
-      <c r="Y17" s="25"/>
-      <c r="Z17" s="25"/>
-      <c r="AA17" s="25"/>
-      <c r="AB17" s="26"/>
-    </row>
-    <row r="18" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="30"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="34" t="s">
-        <v>93</v>
       </c>
       <c r="K18" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L18" s="9"/>
-      <c r="M18" s="35" t="s">
-        <v>94</v>
+      <c r="M18" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="N18" s="8" t="s">
         <v>38</v>
@@ -1793,58 +1763,58 @@
       <c r="AB18" s="9"/>
     </row>
     <row r="19" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="32"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="20" t="s">
+      <c r="A19" s="31"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="K19" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="L19" s="18"/>
+      <c r="M19" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="K19" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="L19" s="19"/>
-      <c r="M19" s="36" t="s">
+      <c r="N19" s="17"/>
+      <c r="O19" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="18"/>
+      <c r="U19" s="34"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="18"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="17"/>
+      <c r="AA19" s="17"/>
+      <c r="AB19" s="18"/>
+    </row>
+    <row r="20" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="N19" s="18"/>
-      <c r="O19" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="37"/>
-      <c r="V19" s="18"/>
-      <c r="W19" s="18"/>
-      <c r="X19" s="19"/>
-      <c r="Y19" s="18"/>
-      <c r="Z19" s="18"/>
-      <c r="AA19" s="18"/>
-      <c r="AB19" s="19"/>
-    </row>
-    <row r="20" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="34" t="s">
+      <c r="B20" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="C20" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="E20" t="s">
         <v>99</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" s="8" t="s">
         <v>100</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>101</v>
       </c>
       <c r="I20" s="9"/>
       <c r="L20" s="9"/>
@@ -1855,31 +1825,31 @@
     </row>
     <row r="21" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I21" s="9"/>
-      <c r="J21" s="34" t="s">
-        <v>70</v>
+      <c r="J21" s="14" t="s">
+        <v>69</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L21" s="9"/>
-      <c r="M21" s="35" t="s">
+      <c r="M21" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="N21" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="O21" s="8" t="s">
         <v>102</v>
-      </c>
-      <c r="N21" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="O21" s="8" t="s">
-        <v>103</v>
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="R21" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S21" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T21" s="9"/>
       <c r="X21" s="9"/>
@@ -1887,18 +1857,18 @@
     </row>
     <row r="22" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I22" s="9"/>
-      <c r="J22" s="34" t="s">
+      <c r="J22" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="K22" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="K22" s="8" t="s">
+      <c r="L22" s="9"/>
+      <c r="M22" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="L22" s="9"/>
-      <c r="M22" s="35" t="s">
-        <v>107</v>
-      </c>
       <c r="O22" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P22" s="9"/>
       <c r="T22" s="9"/>
@@ -1907,18 +1877,18 @@
     </row>
     <row r="23" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I23" s="9"/>
-      <c r="J23" s="34" t="s">
+      <c r="J23" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="K23" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="K23" s="8" t="s">
-        <v>109</v>
-      </c>
       <c r="L23" s="9"/>
-      <c r="M23" s="35" t="s">
-        <v>110</v>
+      <c r="M23" s="13" t="s">
+        <v>139</v>
       </c>
       <c r="O23" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P23" s="9"/>
       <c r="T23" s="9"/>
@@ -1926,22 +1896,22 @@
       <c r="AB23" s="9"/>
     </row>
     <row r="24" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="34" t="s">
-        <v>111</v>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="14" t="s">
+        <v>109</v>
       </c>
       <c r="K24" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="L24" s="9"/>
+      <c r="M24" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="L24" s="9"/>
-      <c r="M24" s="35" t="s">
-        <v>75</v>
-      </c>
       <c r="O24" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P24" s="9"/>
       <c r="T24" s="9"/>
@@ -1949,58 +1919,58 @@
       <c r="AB24" s="9"/>
     </row>
     <row r="25" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" s="25" t="s">
+      <c r="A25" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="24"/>
+      <c r="E25" t="s">
         <v>112</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="D25" s="25"/>
-      <c r="E25" t="s">
-        <v>114</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="25" t="s">
-        <v>78</v>
+      <c r="H25" s="24" t="s">
+        <v>77</v>
       </c>
       <c r="I25" s="9"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="25"/>
-      <c r="T25" s="26"/>
-      <c r="U25" s="33"/>
-      <c r="V25" s="25"/>
-      <c r="W25" s="25"/>
-      <c r="X25" s="26"/>
-      <c r="Y25" s="25"/>
-      <c r="Z25" s="25"/>
-      <c r="AA25" s="25"/>
-      <c r="AB25" s="26"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="24"/>
+      <c r="T25" s="25"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="24"/>
+      <c r="W25" s="24"/>
+      <c r="X25" s="25"/>
+      <c r="Y25" s="24"/>
+      <c r="Z25" s="24"/>
+      <c r="AA25" s="24"/>
+      <c r="AB25" s="25"/>
     </row>
     <row r="26" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="30"/>
+      <c r="A26" s="29"/>
       <c r="I26" s="9"/>
-      <c r="J26" s="34" t="s">
-        <v>93</v>
+      <c r="J26" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="K26" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L26" s="9"/>
-      <c r="M26" s="35" t="s">
-        <v>115</v>
+      <c r="M26" s="13" t="s">
+        <v>113</v>
       </c>
       <c r="N26" s="8" t="s">
         <v>38</v>
@@ -2009,54 +1979,54 @@
         <v>39</v>
       </c>
       <c r="P26" s="9"/>
-      <c r="Q26" s="34" t="s">
-        <v>116</v>
+      <c r="Q26" s="14" t="s">
+        <v>114</v>
       </c>
       <c r="R26" s="8" t="s">
         <v>38</v>
       </c>
       <c r="S26" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T26" s="9"/>
       <c r="X26" s="9"/>
       <c r="AB26" s="9"/>
     </row>
     <row r="27" spans="1:28" ht="171.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="30"/>
+      <c r="A27" s="29"/>
       <c r="I27" s="9"/>
-      <c r="J27" s="34" t="s">
-        <v>117</v>
+      <c r="J27" s="14" t="s">
+        <v>115</v>
       </c>
       <c r="K27" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L27" s="9"/>
-      <c r="M27" s="35" t="s">
-        <v>118</v>
+      <c r="M27" s="13" t="s">
+        <v>116</v>
       </c>
       <c r="N27" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O27" s="8" t="s">
         <v>39</v>
       </c>
       <c r="P27" s="9"/>
-      <c r="Q27" s="34" t="s">
-        <v>119</v>
+      <c r="Q27" s="14" t="s">
+        <v>117</v>
       </c>
       <c r="R27" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S27" s="8" t="s">
         <v>39</v>
       </c>
       <c r="T27" s="9"/>
-      <c r="U27" s="35" t="s">
-        <v>119</v>
+      <c r="U27" s="13" t="s">
+        <v>117</v>
       </c>
       <c r="V27" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W27" s="8" t="s">
         <v>39</v>
@@ -2065,17 +2035,17 @@
       <c r="AB27" s="9"/>
     </row>
     <row r="28" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="30"/>
+      <c r="A28" s="29"/>
       <c r="I28" s="9"/>
-      <c r="J28" s="34" t="s">
-        <v>120</v>
+      <c r="J28" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L28" s="9"/>
-      <c r="M28" s="35" t="s">
-        <v>121</v>
+      <c r="M28" s="13" t="s">
+        <v>119</v>
       </c>
       <c r="O28" s="8" t="s">
         <v>39</v>
@@ -2086,17 +2056,17 @@
       <c r="AB28" s="9"/>
     </row>
     <row r="29" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="30"/>
+      <c r="A29" s="29"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="34" t="s">
+      <c r="J29" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="L29" s="9"/>
+      <c r="M29" s="13" t="s">
         <v>122</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="L29" s="9"/>
-      <c r="M29" s="35" t="s">
-        <v>124</v>
       </c>
       <c r="O29" s="8" t="s">
         <v>39</v>
@@ -2107,30 +2077,30 @@
       <c r="AB29" s="9"/>
     </row>
     <row r="30" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="30"/>
+      <c r="A30" s="29"/>
       <c r="I30" s="9"/>
-      <c r="J30" s="34" t="s">
+      <c r="J30" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="L30" s="9"/>
+      <c r="M30" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="K30" s="8" t="s">
+      <c r="O30" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="L30" s="9"/>
-      <c r="M30" s="35" t="s">
-        <v>127</v>
-      </c>
-      <c r="O30" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="34" t="s">
-        <v>128</v>
-      </c>
       <c r="S30" s="8" t="s">
         <v>39</v>
       </c>
       <c r="T30" s="9"/>
-      <c r="U30" s="39">
+      <c r="U30" s="36">
         <v>2022</v>
       </c>
       <c r="W30" s="8" t="s">
@@ -2140,55 +2110,55 @@
       <c r="AB30" s="9"/>
     </row>
     <row r="31" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="32"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="K31" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="L31" s="19"/>
-      <c r="M31" s="40">
+      <c r="A31" s="31"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="K31" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="L31" s="18"/>
+      <c r="M31" s="37">
         <v>4711</v>
       </c>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="P31" s="19"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
-      <c r="T31" s="19"/>
-      <c r="U31" s="37"/>
-      <c r="V31" s="18"/>
-      <c r="W31" s="18"/>
-      <c r="X31" s="19"/>
-      <c r="Y31" s="18"/>
-      <c r="Z31" s="18"/>
-      <c r="AA31" s="18"/>
-      <c r="AB31" s="19"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
+      <c r="T31" s="18"/>
+      <c r="U31" s="34"/>
+      <c r="V31" s="17"/>
+      <c r="W31" s="17"/>
+      <c r="X31" s="18"/>
+      <c r="Y31" s="17"/>
+      <c r="Z31" s="17"/>
+      <c r="AA31" s="17"/>
+      <c r="AB31" s="18"/>
     </row>
     <row r="32" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="D32" s="24" t="s">
         <v>132</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>134</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>34</v>
@@ -2203,17 +2173,17 @@
     <row r="33" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I33" s="9"/>
       <c r="J33" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>37</v>
       </c>
       <c r="L33" s="9"/>
       <c r="M33" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O33" s="8" t="s">
         <v>39</v>
@@ -2223,24 +2193,24 @@
       <c r="X33" s="9"/>
       <c r="AB33" s="9"/>
       <c r="AD33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="19"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="18"/>
       <c r="J34" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L34" s="9"/>
       <c r="M34" s="12" t="s">
@@ -2251,7 +2221,7 @@
       </c>
       <c r="P34" s="9"/>
       <c r="Q34" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S34" s="8" t="s">
         <v>39</v>
@@ -2265,62 +2235,62 @@
     </row>
     <row r="35" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="33"/>
-      <c r="N35" s="25"/>
-      <c r="O35" s="25"/>
-      <c r="P35" s="25"/>
-      <c r="Q35" s="25"/>
-      <c r="R35" s="25"/>
-      <c r="S35" s="25"/>
-      <c r="T35" s="25"/>
-      <c r="U35" s="33"/>
-      <c r="V35" s="25"/>
-      <c r="W35" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="X35" s="25"/>
-      <c r="Y35" s="25"/>
-      <c r="Z35" s="25"/>
-      <c r="AA35" s="25"/>
-      <c r="AB35" s="25"/>
+        <v>136</v>
+      </c>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="24"/>
+      <c r="O35" s="24"/>
+      <c r="P35" s="24"/>
+      <c r="Q35" s="24"/>
+      <c r="R35" s="24"/>
+      <c r="S35" s="24"/>
+      <c r="T35" s="24"/>
+      <c r="U35" s="32"/>
+      <c r="V35" s="24"/>
+      <c r="W35" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="X35" s="24"/>
+      <c r="Y35" s="24"/>
+      <c r="Z35" s="24"/>
+      <c r="AA35" s="24"/>
+      <c r="AB35" s="24"/>
       <c r="AC35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:30" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="42" t="s">
+    <row r="36" spans="1:30" s="38" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="M36" s="40"/>
+      <c r="U36" s="40"/>
+    </row>
+    <row r="37" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="C36" s="43" t="s">
-        <v>139</v>
-      </c>
-      <c r="D36" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="M36" s="44"/>
-      <c r="U36" s="44"/>
-    </row>
-    <row r="37" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="45" t="s">
-        <v>140</v>
-      </c>
       <c r="E37" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AD38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2328,15 +2298,15 @@
     <row r="41" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C43" s="46"/>
+      <c r="C43" s="41"/>
     </row>
     <row r="44" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="46"/>
+      <c r="C45" s="41"/>
     </row>
     <row r="46" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="46"/>
+      <c r="C47" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
chore: change default permissions to new standard (RDU-48) (#1180)
</commit_message>
<xml_diff>
--- a/testdata/excel2xml/excel2xml-testdata.xlsx
+++ b/testdata/excel2xml/excel2xml-testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/dsp-tools/testdata/excel2xml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DC22B7-1B52-8B49-9009-6393276A79D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178FADB9-1713-B945-A80A-77B184A8CA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="760" windowWidth="29080" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,12 +18,25 @@
   <definedNames>
     <definedName name="example" localSheetId="0">Sheet1!$A$1:$PF$35</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="138">
   <si>
     <t>id</t>
   </si>
@@ -127,9 +140,6 @@
     <t>1999-12-31T23:59:59.9999999+01:00</t>
   </si>
   <si>
-    <t>res-default</t>
-  </si>
-  <si>
     <t xml:space="preserve">         </t>
   </si>
   <si>
@@ -142,9 +152,6 @@
     <t>utf8</t>
   </si>
   <si>
-    <t>prop-default</t>
-  </si>
-  <si>
     <t>Ὅμηρος</t>
   </si>
   <si>
@@ -325,13 +332,7 @@
     <t>http://rdfh.ch/4123/54SYvWF0QUW6a</t>
   </si>
   <si>
-    <t>res-restricted</t>
-  </si>
-  <si>
     <t>This is an annotation to Testthing.</t>
-  </si>
-  <si>
-    <t>prop-restricted</t>
   </si>
   <si>
     <t>Second comment</t>
@@ -456,6 +457,12 @@
   </si>
   <si>
     <t>{"type": "rectangle", "lineWidth": 2, "points": [{"x": 0.08, "y": 0.16}, {"x": 0.73, "y": 0.72}], "original_index": 0}</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>restricted</t>
   </si>
 </sst>
 </file>
@@ -1071,8 +1078,8 @@
   </sheetPr>
   <dimension ref="A1:AI47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1219,7 +1226,7 @@
         <v>33</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>34</v>
+        <v>136</v>
       </c>
       <c r="I2" s="9"/>
       <c r="L2" s="9"/>
@@ -1228,46 +1235,46 @@
       <c r="X2" s="9"/>
       <c r="AB2" s="9"/>
       <c r="AD2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I3" s="9"/>
       <c r="J3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="L3" s="9"/>
       <c r="M3" s="12" t="s">
         <v>32</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P3" s="9"/>
       <c r="Q3" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="T3" s="9"/>
       <c r="U3" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="V3" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="X3" s="9"/>
       <c r="Y3" s="8"/>
@@ -1281,152 +1288,152 @@
     <row r="4" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I4" s="9"/>
       <c r="J4" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L4" s="9"/>
       <c r="M4" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="T4" s="9"/>
       <c r="U4" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="X4" s="9"/>
       <c r="Y4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AA4" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="AB4" s="9"/>
     </row>
     <row r="5" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I5" s="9"/>
       <c r="J5" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P5" s="9"/>
       <c r="Q5" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="T5" s="9"/>
       <c r="U5" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="W5" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="X5" s="9"/>
       <c r="Y5" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AA5" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="AB5" s="9"/>
     </row>
     <row r="6" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I6" s="9"/>
       <c r="J6" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P6" s="9"/>
       <c r="Q6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="T6" s="9"/>
       <c r="U6" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="W6" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="X6" s="9"/>
       <c r="Y6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AA6" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="AB6" s="9"/>
     </row>
     <row r="7" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I7" s="9"/>
       <c r="J7" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L7" s="9"/>
       <c r="M7" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P7" s="9"/>
       <c r="Q7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="S7" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="T7" s="9"/>
       <c r="U7" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="W7" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="X7" s="9"/>
       <c r="Y7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AA7" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="AB7" s="9"/>
     </row>
@@ -1441,18 +1448,18 @@
       <c r="H8" s="17"/>
       <c r="I8" s="18"/>
       <c r="J8" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L8" s="18"/>
       <c r="M8" s="20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N8" s="17"/>
       <c r="O8" s="17" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P8" s="18"/>
       <c r="Q8" s="21"/>
@@ -1470,16 +1477,16 @@
     </row>
     <row r="9" spans="1:35" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="G9" s="8" t="s">
-        <v>34</v>
+        <v>136</v>
       </c>
       <c r="I9" s="9"/>
       <c r="L9" s="9"/>
@@ -1491,26 +1498,26 @@
         <v>29</v>
       </c>
       <c r="AG9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I10" s="9"/>
       <c r="J10" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L10" s="9"/>
       <c r="M10" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P10" s="9"/>
       <c r="T10" s="9"/>
@@ -1528,17 +1535,17 @@
       <c r="H11" s="17"/>
       <c r="I11" s="18"/>
       <c r="J11" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L11" s="9"/>
       <c r="M11" s="12" t="s">
         <v>30</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P11" s="9"/>
       <c r="T11" s="9"/>
@@ -1547,22 +1554,22 @@
     </row>
     <row r="12" spans="1:35" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="G12" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="H12" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>77</v>
-      </c>
       <c r="I12" s="9" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="J12" s="24"/>
       <c r="K12" s="24"/>
@@ -1587,20 +1594,20 @@
     <row r="13" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I13" s="9"/>
       <c r="J13" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L13" s="9"/>
       <c r="M13" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O13" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P13" s="9"/>
       <c r="Q13" s="29"/>
@@ -1610,26 +1617,26 @@
       <c r="Y13" s="29"/>
       <c r="AB13" s="9"/>
       <c r="AC13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I14" s="9"/>
       <c r="J14" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P14" s="9"/>
       <c r="Q14" s="29"/>
@@ -1642,20 +1649,20 @@
     <row r="15" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I15" s="9"/>
       <c r="J15" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P15" s="9"/>
       <c r="Q15" s="29"/>
@@ -1669,20 +1676,20 @@
       <c r="H16" s="17"/>
       <c r="I16" s="18"/>
       <c r="J16" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="K16" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="L16" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="K16" s="17" t="s">
+      <c r="M16" s="30" t="s">
         <v>85</v>
-      </c>
-      <c r="L16" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="M16" s="30" t="s">
-        <v>87</v>
       </c>
       <c r="N16" s="17"/>
       <c r="O16" s="17" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P16" s="18"/>
       <c r="Q16" s="31"/>
@@ -1700,21 +1707,21 @@
     </row>
     <row r="17" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="D17" s="24" t="s">
         <v>89</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>91</v>
       </c>
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
       <c r="G17" s="24" t="s">
-        <v>34</v>
+        <v>136</v>
       </c>
       <c r="H17" s="24"/>
       <c r="I17" s="9"/>
@@ -1742,20 +1749,20 @@
       <c r="A18" s="29"/>
       <c r="I18" s="9"/>
       <c r="J18" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P18" s="9"/>
       <c r="T18" s="9"/>
@@ -1773,18 +1780,18 @@
       <c r="H19" s="17"/>
       <c r="I19" s="18"/>
       <c r="J19" s="19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L19" s="18"/>
       <c r="M19" s="33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="N19" s="17"/>
       <c r="O19" s="19" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P19" s="18"/>
       <c r="Q19" s="17"/>
@@ -1802,19 +1809,19 @@
     </row>
     <row r="20" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="E20" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" t="s">
-        <v>99</v>
-      </c>
       <c r="G20" s="8" t="s">
-        <v>100</v>
+        <v>137</v>
       </c>
       <c r="I20" s="9"/>
       <c r="L20" s="9"/>
@@ -1826,30 +1833,30 @@
     <row r="21" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I21" s="9"/>
       <c r="J21" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L21" s="9"/>
       <c r="M21" s="13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O21" s="8" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="R21" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="S21" s="8" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="T21" s="9"/>
       <c r="X21" s="9"/>
@@ -1858,17 +1865,17 @@
     <row r="22" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I22" s="9"/>
       <c r="J22" s="14" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="L22" s="9"/>
       <c r="M22" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="O22" s="8" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="P22" s="9"/>
       <c r="T22" s="9"/>
@@ -1878,17 +1885,17 @@
     <row r="23" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I23" s="9"/>
       <c r="J23" s="14" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="L23" s="9"/>
       <c r="M23" s="13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="O23" s="8" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="P23" s="9"/>
       <c r="T23" s="9"/>
@@ -1901,17 +1908,17 @@
       <c r="G24" s="17"/>
       <c r="I24" s="18"/>
       <c r="J24" s="14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L24" s="9"/>
       <c r="M24" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="O24" s="8" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="P24" s="9"/>
       <c r="T24" s="9"/>
@@ -1920,23 +1927,23 @@
     </row>
     <row r="25" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D25" s="24"/>
       <c r="E25" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>34</v>
+        <v>136</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="24"/>
@@ -1963,30 +1970,30 @@
       <c r="A26" s="29"/>
       <c r="I26" s="9"/>
       <c r="J26" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L26" s="9"/>
       <c r="M26" s="13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P26" s="9"/>
       <c r="Q26" s="14" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="R26" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S26" s="8" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="T26" s="9"/>
       <c r="X26" s="9"/>
@@ -1996,40 +2003,40 @@
       <c r="A27" s="29"/>
       <c r="I27" s="9"/>
       <c r="J27" s="14" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L27" s="9"/>
       <c r="M27" s="13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="N27" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P27" s="9"/>
       <c r="Q27" s="14" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="R27" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="S27" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="T27" s="9"/>
       <c r="U27" s="13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="V27" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="W27" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="X27" s="9"/>
       <c r="AB27" s="9"/>
@@ -2038,17 +2045,17 @@
       <c r="A28" s="29"/>
       <c r="I28" s="9"/>
       <c r="J28" s="14" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L28" s="9"/>
       <c r="M28" s="13" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="O28" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P28" s="9"/>
       <c r="T28" s="9"/>
@@ -2059,17 +2066,17 @@
       <c r="A29" s="29"/>
       <c r="I29" s="9"/>
       <c r="J29" s="14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="L29" s="9"/>
       <c r="M29" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="O29" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P29" s="9"/>
       <c r="T29" s="9"/>
@@ -2080,31 +2087,31 @@
       <c r="A30" s="29"/>
       <c r="I30" s="9"/>
       <c r="J30" s="14" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="L30" s="9"/>
       <c r="M30" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P30" s="9"/>
       <c r="Q30" s="14" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="S30" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="T30" s="9"/>
       <c r="U30" s="36">
         <v>2022</v>
       </c>
       <c r="W30" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="X30" s="9"/>
       <c r="AB30" s="9"/>
@@ -2120,10 +2127,10 @@
       <c r="H31" s="17"/>
       <c r="I31" s="18"/>
       <c r="J31" s="19" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K31" s="17" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="L31" s="18"/>
       <c r="M31" s="37">
@@ -2131,7 +2138,7 @@
       </c>
       <c r="N31" s="17"/>
       <c r="O31" s="17" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P31" s="18"/>
       <c r="Q31" s="17"/>
@@ -2149,19 +2156,19 @@
     </row>
     <row r="32" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>34</v>
+        <v>136</v>
       </c>
       <c r="I32" s="9"/>
       <c r="L32" s="9"/>
@@ -2173,27 +2180,27 @@
     <row r="33" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I33" s="9"/>
       <c r="J33" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L33" s="9"/>
       <c r="M33" s="12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O33" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P33" s="9"/>
       <c r="T33" s="9"/>
       <c r="X33" s="9"/>
       <c r="AB33" s="9"/>
       <c r="AD33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2207,38 +2214,38 @@
       <c r="H34" s="17"/>
       <c r="I34" s="18"/>
       <c r="J34" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L34" s="9"/>
       <c r="M34" s="12" t="s">
         <v>30</v>
       </c>
       <c r="O34" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="P34" s="9"/>
       <c r="Q34" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S34" s="8" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="T34" s="9"/>
       <c r="X34" s="9"/>
       <c r="AB34" s="9"/>
       <c r="AC34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H35" s="24"/>
       <c r="I35" s="24"/>
@@ -2256,7 +2263,7 @@
       <c r="U35" s="32"/>
       <c r="V35" s="24"/>
       <c r="W35" s="24" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="X35" s="24"/>
       <c r="Y35" s="24"/>
@@ -2269,28 +2276,28 @@
     </row>
     <row r="36" spans="1:30" s="38" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="39" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D36" s="39" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="M36" s="40"/>
       <c r="U36" s="40"/>
     </row>
     <row r="37" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C37" s="41" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E37" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AD38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat!: remove support for knora-base:Annotation (DEV-4430) (#1314)
Co-authored-by: Nora-Olivia-Ammann <103038637+Nora-Olivia-Ammann@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/testdata/excel2xml/excel2xml-testdata.xlsx
+++ b/testdata/excel2xml/excel2xml-testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/dsp-tools/testdata/excel2xml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178FADB9-1713-B945-A80A-77B184A8CA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B6EAC4-A784-4549-B6D1-AFCBD5F7E996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="760" windowWidth="29080" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="example" localSheetId="0">Sheet1!$A$1:$PF$35</definedName>
+    <definedName name="example" localSheetId="0">Sheet1!$A$1:$PF$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="133">
   <si>
     <t>id</t>
   </si>
@@ -227,28 +227,13 @@
     <t>https://www.ancestry.com/discoveryui-content/view/47577828:60525?ssrc=pt&amp;tid=109007397&amp;pid=410070328478</t>
   </si>
   <si>
-    <t>annotation_0</t>
-  </si>
-  <si>
-    <t>Annotation</t>
-  </si>
-  <si>
-    <t>Annotation to Homer</t>
-  </si>
-  <si>
     <t xml:space="preserve">        </t>
   </si>
   <si>
     <t>hasComment</t>
   </si>
   <si>
-    <t>This is an annotation to the resource Homer</t>
-  </si>
-  <si>
     <t>xml</t>
-  </si>
-  <si>
-    <t>isAnnotationOf</t>
   </si>
   <si>
     <t>resptr-prop</t>
@@ -1076,10 +1061,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AI47"/>
+  <dimension ref="A1:AI44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1226,7 +1211,7 @@
         <v>33</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="I2" s="9"/>
       <c r="L2" s="9"/>
@@ -1254,7 +1239,7 @@
         <v>37</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P3" s="9"/>
       <c r="Q3" s="8" t="s">
@@ -1264,7 +1249,7 @@
         <v>37</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="T3" s="9"/>
       <c r="U3" s="12" t="s">
@@ -1274,7 +1259,7 @@
         <v>37</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="X3" s="9"/>
       <c r="Y3" s="8"/>
@@ -1298,28 +1283,28 @@
         <v>42</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="14" t="s">
         <v>43</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="T4" s="9"/>
       <c r="U4" s="13" t="s">
         <v>44</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="X4" s="9"/>
       <c r="Y4" t="s">
         <v>45</v>
       </c>
       <c r="AA4" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AB4" s="9"/>
     </row>
@@ -1336,28 +1321,28 @@
         <v>47</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P5" s="9"/>
       <c r="Q5" s="15" t="s">
         <v>48</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="T5" s="9"/>
       <c r="U5" s="16" t="s">
         <v>49</v>
       </c>
       <c r="W5" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="X5" s="9"/>
       <c r="Y5" s="15" t="s">
         <v>50</v>
       </c>
       <c r="AA5" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AB5" s="9"/>
     </row>
@@ -1374,28 +1359,28 @@
         <v>52</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P6" s="9"/>
       <c r="Q6" t="s">
         <v>53</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="T6" s="9"/>
       <c r="U6" s="16" t="s">
         <v>54</v>
       </c>
       <c r="W6" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="X6" s="9"/>
       <c r="Y6" t="s">
         <v>55</v>
       </c>
       <c r="AA6" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AB6" s="9"/>
     </row>
@@ -1412,32 +1397,32 @@
         <v>57</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P7" s="9"/>
       <c r="Q7" t="s">
         <v>58</v>
       </c>
       <c r="S7" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="T7" s="9"/>
       <c r="U7" s="13" t="s">
         <v>59</v>
       </c>
       <c r="W7" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="X7" s="9"/>
       <c r="Y7" t="s">
         <v>60</v>
       </c>
       <c r="AA7" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AB7" s="9"/>
     </row>
-    <row r="8" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -1459,7 +1444,7 @@
       </c>
       <c r="N8" s="17"/>
       <c r="O8" s="17" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P8" s="18"/>
       <c r="Q8" s="21"/>
@@ -1477,647 +1462,657 @@
     </row>
     <row r="9" spans="1:35" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="I9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="X9" s="9"/>
-      <c r="AB9" s="9"/>
-      <c r="AD9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>66</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="26"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="27"/>
+      <c r="Z9" s="24"/>
+      <c r="AA9" s="24"/>
+      <c r="AB9" s="25"/>
     </row>
     <row r="10" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I10" s="9"/>
       <c r="J10" s="8" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>36</v>
       </c>
       <c r="L10" s="9"/>
-      <c r="M10" s="12" t="s">
-        <v>68</v>
+      <c r="M10" s="28" t="s">
+        <v>72</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P10" s="9"/>
+      <c r="Q10" s="29"/>
       <c r="T10" s="9"/>
+      <c r="U10" s="28"/>
       <c r="X10" s="9"/>
+      <c r="Y10" s="29"/>
       <c r="AB10" s="9"/>
+      <c r="AC10" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="18"/>
+      <c r="I11" s="9"/>
       <c r="J11" s="8" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="L11" s="9"/>
-      <c r="M11" s="12" t="s">
-        <v>30</v>
+      <c r="M11" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P11" s="9"/>
+      <c r="Q11" s="29"/>
       <c r="T11" s="9"/>
+      <c r="U11" s="28"/>
       <c r="X11" s="9"/>
+      <c r="Y11" s="29"/>
       <c r="AB11" s="9"/>
     </row>
-    <row r="12" spans="1:35" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="H12" s="24" t="s">
+    <row r="12" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I12" s="9"/>
+      <c r="J12" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="25"/>
-      <c r="U12" s="26"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="24"/>
-      <c r="X12" s="25"/>
-      <c r="Y12" s="27"/>
-      <c r="Z12" s="24"/>
-      <c r="AA12" s="24"/>
-      <c r="AB12" s="25"/>
+      <c r="K12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="9"/>
+      <c r="M12" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="29"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="28"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="29"/>
+      <c r="AB12" s="9"/>
     </row>
     <row r="13" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I13" s="9"/>
-      <c r="J13" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="L13" s="9"/>
-      <c r="M13" s="28" t="s">
+      <c r="H13" s="17"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="N13" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="O13" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="29"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="28"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="29"/>
-      <c r="AB13" s="9"/>
-      <c r="AC13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K13" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="M13" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="18"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="31"/>
+      <c r="Z13" s="17"/>
+      <c r="AA13" s="17"/>
+      <c r="AB13" s="18"/>
+    </row>
+    <row r="14" spans="1:35" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="H14" s="24"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="L14" s="9"/>
-      <c r="M14" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="O14" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="29"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="28"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="29"/>
-      <c r="AB14" s="9"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="25"/>
+      <c r="Y14" s="24"/>
+      <c r="Z14" s="24"/>
+      <c r="AA14" s="24"/>
+      <c r="AB14" s="25"/>
     </row>
     <row r="15" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="29"/>
       <c r="I15" s="9"/>
-      <c r="J15" s="8" t="s">
-        <v>80</v>
+      <c r="J15" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>36</v>
       </c>
       <c r="L15" s="9"/>
-      <c r="M15" s="28" t="s">
-        <v>81</v>
+      <c r="M15" s="13" t="s">
+        <v>86</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P15" s="9"/>
-      <c r="Q15" s="29"/>
       <c r="T15" s="9"/>
-      <c r="U15" s="28"/>
       <c r="X15" s="9"/>
-      <c r="Y15" s="29"/>
       <c r="AB15" s="9"/>
     </row>
-    <row r="16" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="31"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="18"/>
-      <c r="J16" s="17" t="s">
-        <v>82</v>
+      <c r="J16" s="19" t="s">
+        <v>87</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="L16" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="M16" s="30" t="s">
-        <v>85</v>
+        <v>66</v>
+      </c>
+      <c r="L16" s="18"/>
+      <c r="M16" s="33" t="s">
+        <v>88</v>
       </c>
       <c r="N16" s="17"/>
-      <c r="O16" s="17" t="s">
-        <v>136</v>
+      <c r="O16" s="19" t="s">
+        <v>131</v>
       </c>
       <c r="P16" s="18"/>
-      <c r="Q16" s="31"/>
+      <c r="Q16" s="17"/>
       <c r="R16" s="17"/>
       <c r="S16" s="17"/>
       <c r="T16" s="18"/>
-      <c r="U16" s="30"/>
+      <c r="U16" s="34"/>
       <c r="V16" s="17"/>
       <c r="W16" s="17"/>
       <c r="X16" s="18"/>
-      <c r="Y16" s="31"/>
+      <c r="Y16" s="17"/>
       <c r="Z16" s="17"/>
       <c r="AA16" s="17"/>
       <c r="AB16" s="18"/>
     </row>
-    <row r="17" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" s="24" t="s">
+    <row r="17" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="H17" s="24"/>
+      <c r="B17" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>132</v>
+      </c>
       <c r="I17" s="9"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="25"/>
-      <c r="U17" s="32"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="24"/>
-      <c r="X17" s="25"/>
-      <c r="Y17" s="24"/>
-      <c r="Z17" s="24"/>
-      <c r="AA17" s="24"/>
-      <c r="AB17" s="25"/>
-    </row>
-    <row r="18" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="29"/>
+      <c r="L17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="AB17" s="9"/>
+    </row>
+    <row r="18" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I18" s="9"/>
       <c r="J18" s="14" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="K18" s="8" t="s">
         <v>36</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="13" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="P18" s="9"/>
+      <c r="Q18" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="R18" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="S18" s="8" t="s">
+        <v>132</v>
+      </c>
       <c r="T18" s="9"/>
       <c r="X18" s="9"/>
       <c r="AB18" s="9"/>
     </row>
-    <row r="19" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="31"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="K19" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="L19" s="18"/>
-      <c r="M19" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="N19" s="17"/>
-      <c r="O19" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="34"/>
-      <c r="V19" s="17"/>
-      <c r="W19" s="17"/>
-      <c r="X19" s="18"/>
-      <c r="Y19" s="17"/>
-      <c r="Z19" s="17"/>
-      <c r="AA19" s="17"/>
-      <c r="AB19" s="18"/>
-    </row>
-    <row r="20" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" s="8" t="s">
+    <row r="19" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I19" s="9"/>
+      <c r="J19" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="K19" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E20" t="s">
+      <c r="L19" s="9"/>
+      <c r="M19" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>137</v>
-      </c>
+      <c r="O19" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="P19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="AB19" s="9"/>
+    </row>
+    <row r="20" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I20" s="9"/>
+      <c r="J20" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>99</v>
+      </c>
       <c r="L20" s="9"/>
+      <c r="M20" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="O20" s="8" t="s">
+        <v>132</v>
+      </c>
       <c r="P20" s="9"/>
       <c r="T20" s="9"/>
       <c r="X20" s="9"/>
       <c r="AB20" s="9"/>
     </row>
-    <row r="21" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I21" s="9"/>
+    <row r="21" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="I21" s="18"/>
       <c r="J21" s="14" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="L21" s="9"/>
       <c r="M21" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="N21" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O21" s="8" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="P21" s="9"/>
-      <c r="Q21" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="R21" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="S21" s="8" t="s">
-        <v>137</v>
-      </c>
       <c r="T21" s="9"/>
       <c r="X21" s="9"/>
       <c r="AB21" s="9"/>
     </row>
-    <row r="22" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" t="s">
+        <v>103</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>70</v>
+      </c>
       <c r="I22" s="9"/>
-      <c r="J22" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="L22" s="9"/>
-      <c r="M22" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="O22" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="P22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="X22" s="9"/>
-      <c r="AB22" s="9"/>
-    </row>
-    <row r="23" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="25"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="25"/>
+      <c r="U22" s="32"/>
+      <c r="V22" s="24"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="25"/>
+      <c r="Y22" s="24"/>
+      <c r="Z22" s="24"/>
+      <c r="AA22" s="24"/>
+      <c r="AB22" s="25"/>
+    </row>
+    <row r="23" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="29"/>
       <c r="I23" s="9"/>
       <c r="J23" s="14" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>104</v>
+        <v>36</v>
       </c>
       <c r="L23" s="9"/>
       <c r="M23" s="13" t="s">
-        <v>135</v>
+        <v>104</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="O23" s="8" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="P23" s="9"/>
+      <c r="Q23" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="R23" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="S23" s="8" t="s">
+        <v>132</v>
+      </c>
       <c r="T23" s="9"/>
       <c r="X23" s="9"/>
       <c r="AB23" s="9"/>
     </row>
-    <row r="24" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="I24" s="18"/>
+    <row r="24" spans="1:30" ht="171.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="29"/>
+      <c r="I24" s="9"/>
       <c r="J24" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="L24" s="9"/>
       <c r="M24" s="13" t="s">
-        <v>72</v>
+        <v>107</v>
+      </c>
+      <c r="N24" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="O24" s="8" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="P24" s="9"/>
+      <c r="Q24" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="R24" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="S24" s="8" t="s">
+        <v>131</v>
+      </c>
       <c r="T24" s="9"/>
+      <c r="U24" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="V24" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="W24" s="8" t="s">
+        <v>131</v>
+      </c>
       <c r="X24" s="9"/>
       <c r="AB24" s="9"/>
     </row>
-    <row r="25" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" s="24"/>
-      <c r="E25" t="s">
-        <v>108</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="H25" s="24" t="s">
-        <v>75</v>
-      </c>
+    <row r="25" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="29"/>
       <c r="I25" s="9"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="24"/>
-      <c r="S25" s="24"/>
-      <c r="T25" s="25"/>
-      <c r="U25" s="32"/>
-      <c r="V25" s="24"/>
-      <c r="W25" s="24"/>
-      <c r="X25" s="25"/>
-      <c r="Y25" s="24"/>
-      <c r="Z25" s="24"/>
-      <c r="AA25" s="24"/>
-      <c r="AB25" s="25"/>
-    </row>
-    <row r="26" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J25" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L25" s="9"/>
+      <c r="M25" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="O25" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="P25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="AB25" s="9"/>
+    </row>
+    <row r="26" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="29"/>
       <c r="I26" s="9"/>
       <c r="J26" s="14" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="L26" s="9"/>
       <c r="M26" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="N26" s="8" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P26" s="9"/>
-      <c r="Q26" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="R26" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="S26" s="8" t="s">
-        <v>137</v>
-      </c>
       <c r="T26" s="9"/>
       <c r="X26" s="9"/>
       <c r="AB26" s="9"/>
     </row>
-    <row r="27" spans="1:28" ht="171.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="29"/>
       <c r="I27" s="9"/>
       <c r="J27" s="14" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="L27" s="9"/>
       <c r="M27" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="N27" s="8" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P27" s="9"/>
       <c r="Q27" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="R27" s="8" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="S27" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="T27" s="9"/>
-      <c r="U27" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="V27" s="8" t="s">
-        <v>69</v>
+      <c r="U27" s="36">
+        <v>2022</v>
       </c>
       <c r="W27" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="X27" s="9"/>
       <c r="AB27" s="9"/>
     </row>
-    <row r="28" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="L28" s="9"/>
-      <c r="M28" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="O28" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="P28" s="9"/>
-      <c r="T28" s="9"/>
-      <c r="X28" s="9"/>
-      <c r="AB28" s="9"/>
-    </row>
-    <row r="29" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="29"/>
+    <row r="28" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="31"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="K28" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="L28" s="18"/>
+      <c r="M28" s="37">
+        <v>4711</v>
+      </c>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="18"/>
+      <c r="U28" s="34"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="18"/>
+      <c r="Y28" s="17"/>
+      <c r="Z28" s="17"/>
+      <c r="AA28" s="17"/>
+      <c r="AB28" s="18"/>
+    </row>
+    <row r="29" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>131</v>
+      </c>
       <c r="I29" s="9"/>
-      <c r="J29" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>117</v>
-      </c>
       <c r="L29" s="9"/>
-      <c r="M29" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="O29" s="8" t="s">
-        <v>136</v>
-      </c>
       <c r="P29" s="9"/>
       <c r="T29" s="9"/>
       <c r="X29" s="9"/>
       <c r="AB29" s="9"/>
     </row>
-    <row r="30" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="29"/>
+    <row r="30" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I30" s="9"/>
-      <c r="J30" s="14" t="s">
-        <v>119</v>
+      <c r="J30" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>120</v>
+        <v>36</v>
       </c>
       <c r="L30" s="9"/>
-      <c r="M30" s="13" t="s">
-        <v>121</v>
+      <c r="M30" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="N30" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="P30" s="9"/>
-      <c r="Q30" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="S30" s="8" t="s">
-        <v>136</v>
-      </c>
       <c r="T30" s="9"/>
-      <c r="U30" s="36">
-        <v>2022</v>
-      </c>
-      <c r="W30" s="8" t="s">
-        <v>136</v>
-      </c>
       <c r="X30" s="9"/>
       <c r="AB30" s="9"/>
-    </row>
-    <row r="31" spans="1:28" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="31"/>
+      <c r="AD30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="17"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -2126,194 +2121,107 @@
       <c r="G31" s="17"/>
       <c r="H31" s="17"/>
       <c r="I31" s="18"/>
-      <c r="J31" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="K31" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="L31" s="18"/>
-      <c r="M31" s="37">
-        <v>4711</v>
-      </c>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="17"/>
-      <c r="R31" s="17"/>
-      <c r="S31" s="17"/>
-      <c r="T31" s="18"/>
-      <c r="U31" s="34"/>
-      <c r="V31" s="17"/>
-      <c r="W31" s="17"/>
-      <c r="X31" s="18"/>
-      <c r="Y31" s="17"/>
-      <c r="Z31" s="17"/>
-      <c r="AA31" s="17"/>
-      <c r="AB31" s="18"/>
-    </row>
-    <row r="32" spans="1:28" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J31" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L31" s="9"/>
+      <c r="M31" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="O31" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="S31" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="T31" s="9"/>
+      <c r="X31" s="9"/>
+      <c r="AB31" s="9"/>
+      <c r="AC31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B32" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="F32" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D32" s="24" t="s">
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="24"/>
+      <c r="S32" s="24"/>
+      <c r="T32" s="24"/>
+      <c r="U32" s="32"/>
+      <c r="V32" s="24"/>
+      <c r="W32" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="X32" s="24"/>
+      <c r="Y32" s="24"/>
+      <c r="Z32" s="24"/>
+      <c r="AA32" s="24"/>
+      <c r="AB32" s="24"/>
+      <c r="AC32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:30" s="38" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="G32" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="I32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="T32" s="9"/>
-      <c r="X32" s="9"/>
-      <c r="AB32" s="9"/>
-    </row>
-    <row r="33" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I33" s="9"/>
-      <c r="J33" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="L33" s="9"/>
-      <c r="M33" s="12" t="s">
+      <c r="D33" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="M33" s="40"/>
+      <c r="U33" s="40"/>
+    </row>
+    <row r="34" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="N33" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="O33" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="P33" s="9"/>
-      <c r="T33" s="9"/>
-      <c r="X33" s="9"/>
-      <c r="AB33" s="9"/>
-      <c r="AD33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="K34" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="L34" s="9"/>
-      <c r="M34" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="O34" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="S34" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="T34" s="9"/>
-      <c r="X34" s="9"/>
-      <c r="AB34" s="9"/>
-      <c r="AC34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="24"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="24"/>
-      <c r="O35" s="24"/>
-      <c r="P35" s="24"/>
-      <c r="Q35" s="24"/>
-      <c r="R35" s="24"/>
-      <c r="S35" s="24"/>
-      <c r="T35" s="24"/>
-      <c r="U35" s="32"/>
-      <c r="V35" s="24"/>
-      <c r="W35" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="X35" s="24"/>
-      <c r="Y35" s="24"/>
-      <c r="Z35" s="24"/>
-      <c r="AA35" s="24"/>
-      <c r="AB35" s="24"/>
-      <c r="AC35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:30" s="38" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="C36" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="D36" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="M36" s="40"/>
-      <c r="U36" s="40"/>
-    </row>
-    <row r="37" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="E37" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="38" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AD38" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C43" s="41"/>
-    </row>
-    <row r="44" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="41"/>
-    </row>
-    <row r="46" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="41"/>
+      <c r="E34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C40" s="41"/>
+    </row>
+    <row r="41" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="41"/>
+    </row>
+    <row r="43" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="2:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C44" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
chore: apply new permissions terminology - everywhere except xmllib (DEV-5077) (#1804)
</commit_message>
<xml_diff>
--- a/testdata/excel2xml/excel2xml-testdata.xlsx
+++ b/testdata/excel2xml/excel2xml-testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/dsp-tools/testdata/excel2xml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B6EAC4-A784-4549-B6D1-AFCBD5F7E996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48F256F-0A53-5B46-8D8B-8BC93BA7B2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="760" windowWidth="29080" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,10 +444,10 @@
     <t>{"type": "rectangle", "lineWidth": 2, "points": [{"x": 0.08, "y": 0.16}, {"x": 0.73, "y": 0.72}], "original_index": 0}</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>restricted</t>
+    <t>public</t>
+  </si>
+  <si>
+    <t>private</t>
   </si>
 </sst>
 </file>
@@ -1063,8 +1063,8 @@
   </sheetPr>
   <dimension ref="A1:AI44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>